<commit_message>
Fixed submit order button
</commit_message>
<xml_diff>
--- a/ID data.xlsx
+++ b/ID data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,27 +475,27 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>19895885</v>
+        <v>19896232</v>
       </c>
       <c r="C2" t="n">
         <v>32001378</v>
       </c>
       <c r="D2" t="n">
-        <v>17917149</v>
+        <v>17917451</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CalRpcPslyBrWmRlxJrsTee-blkhthr-xxl</t>
+          <t>dsc-carptxt-pgcrw-ltblulrg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CalRpcPslyBrWmRlxJrsTee-blkhthr-xxl</t>
+          <t>dsc-carptxt-pgcrw-ltblulrg</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>California Republic Paisley Bear Women's Relaxed Jersey Tee - XX-Large / Black Heather</t>
+          <t>California Repeat Text Pigment Dyed Crewneck Light Blue - Large / Pigment Light Blue</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -507,27 +507,27 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19895886</v>
+        <v>19896260</v>
       </c>
       <c r="C3" t="n">
         <v>32001378</v>
       </c>
       <c r="D3" t="n">
-        <v>17917149</v>
+        <v>17917476</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>sf-surfbear-mug</t>
+          <t>dsc-flgdstrsshdy-med</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>sf-surfbear-mug</t>
+          <t>dsc-flgdstrsshdy-med</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>California Surf Bear Ceramic Mug - Standard / white</t>
+          <t>California State Flag Distressed Vintage Asst Colors Hoodie - Medium / Black</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -539,27 +539,27 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19895887</v>
+        <v>19896261</v>
       </c>
       <c r="C4" t="n">
         <v>32001378</v>
       </c>
       <c r="D4" t="n">
-        <v>17917149</v>
+        <v>17917476</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>sf-pillow</t>
+          <t>dsc-carpblkovrsl-rgln-med</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>sf-pillow</t>
+          <t>dsc-carpblkovrsl-rgln-med</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>I Love You California Bear Plush Pillow - One Size / Brown</t>
+          <t>California Republic Black Oversized Silhouette Raglan Hoodie - Medium / Gunmetal Heather/Black</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -571,27 +571,27 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>19896185</v>
+        <v>19896304</v>
       </c>
       <c r="C5" t="n">
         <v>32001378</v>
       </c>
       <c r="D5" t="n">
-        <v>17917410</v>
+        <v>17917518</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>sf-MntBearPatch</t>
+          <t>140523888</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>sf-MntBearPatch</t>
+          <t>dsc-cr-screenp-trucker-hat-black</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>I Love You Califoria Mountain Bear Patch - One Size / Brown</t>
+          <t>California Republic Screen Print Trucker Hat - Black</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -603,27 +603,27 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>19896186</v>
+        <v>19896305</v>
       </c>
       <c r="C6" t="n">
         <v>32001378</v>
       </c>
       <c r="D6" t="n">
-        <v>17917410</v>
+        <v>17917519</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>dsc-CaSmmrBrHDY-whtxlg</t>
+          <t>dsc-calirpfltcp-blk/wht</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>dsc-CaSmmrBrHDY-whtxlg</t>
+          <t>dsc-calirpfltcp-blk/wht</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>California Summer Surf Bear Sweatshirt Hoodie - X-Large / White</t>
+          <t>California Republic Flag Flat Bill Snapback Mesh Truckers Cap - One size fits most / Black/White</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -635,31 +635,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>19896187</v>
+        <v>19896306</v>
       </c>
       <c r="C7" t="n">
         <v>32001378</v>
       </c>
       <c r="D7" t="n">
-        <v>17917410</v>
+        <v>17917519</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>sf-TeaTwl</t>
+          <t>dsc-caliorg-fb-blk</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>sf-TeaTwl</t>
+          <t>dsc-caliorg-fb-blk</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>I Love You California Tea Towel - One Size / White</t>
+          <t>California Republic Original State Flag Snapback Hat On Black - Flat Bill - One size fits most / Black/White</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -667,27 +667,27 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>19896188</v>
+        <v>19896319</v>
       </c>
       <c r="C8" t="n">
         <v>32001378</v>
       </c>
       <c r="D8" t="n">
-        <v>17917410</v>
+        <v>17917531</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>dsc-CBrOnBkePRMYTH-blksml</t>
+          <t>dsc-trkrcp-blk/wht</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>dsc-CBrOnBkePRMYTH-blksml</t>
+          <t>dsc-trkrcp-blk/wht</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>California Bear On Bike Asst Colors Youth T-Shirt/tee - Small / Black</t>
+          <t>California State Flag Snapback Mesh Truckers Cap - One size fits most / Black/White</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -699,27 +699,27 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>19896189</v>
+        <v>19896477</v>
       </c>
       <c r="C9" t="n">
         <v>32001378</v>
       </c>
       <c r="D9" t="n">
-        <v>17917410</v>
+        <v>17917666</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>dsc-SnFrnCaNenRnbwPRMYTH-blkmed</t>
+          <t>dsc-rtrobldtee-mrnxlg</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>dsc-SnFrnCaNenRnbwPRMYTH-blkmed</t>
+          <t>dsc-rtrobldtee-mrnxlg</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>San Francisco California Neon Rainbow Asst Colors Youth T-Shirt/tee - Medium / Black</t>
+          <t>California Republic Vintage Retro Asst Colors T-shirt/tee - X-Large / Maroon</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -731,27 +731,27 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>19896200</v>
+        <v>19896479</v>
       </c>
       <c r="C10" t="n">
         <v>32001378</v>
       </c>
       <c r="D10" t="n">
-        <v>17917421</v>
+        <v>17917668</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>dsc-mmhpr-blk3xl</t>
+          <t>140524065</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>dsc-mmhpr-blk3xl</t>
+          <t>dsc-CalNo1DmndHDY-rshgrnxxl</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Marilyn Monroe Hot Pink Retro Asst Colors T-shirt/tee - XXX-Large / Black</t>
+          <t>California Republic No. 1 Diamond Hustle Sweatshirt Hoodie - Irish Green XX-Large</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -763,27 +763,27 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19896206</v>
+        <v>19896528</v>
       </c>
       <c r="C11" t="n">
         <v>32001378</v>
       </c>
       <c r="D11" t="n">
-        <v>17917427</v>
+        <v>17917713</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>DSC-BrdlssL/S-wht-XL</t>
+          <t>CaRpBrdrlssBrFlgSPRSFTCRW-mstblu-xl</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>DSC-BrdlssL/S-wht-XL</t>
+          <t>CaRpBrdrlssBrFlgSPRSFTCRW-mstblu-xl</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>California State Flag - Borderless White Long Sleeve T-Shirt - X-Large / White</t>
+          <t>California Republic Borderless Bear Flag Super Soft Crewneck Sweater - X-Large / Misty Blue</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -795,27 +795,27 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>19896229</v>
+        <v>19896578</v>
       </c>
       <c r="C12" t="n">
         <v>32001378</v>
       </c>
       <c r="D12" t="n">
-        <v>17917448</v>
+        <v>17917757</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>dsc-CalArrwBrHDY-whtxlg</t>
+          <t>140524164</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>dsc-CalArrwBrHDY-whtxlg</t>
+          <t>dsc-capoppystckr</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>California Arrow Bear Sweatshirt Hoodie - X-Large / White</t>
+          <t>Life at Sea Sticker (CA Poppy)</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -827,27 +827,27 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19896232</v>
+        <v>19896579</v>
       </c>
       <c r="C13" t="n">
         <v>32001378</v>
       </c>
       <c r="D13" t="n">
-        <v>17917451</v>
+        <v>17917758</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>dsc-carptxt-pgcrw-ltblulrg</t>
+          <t>140524165</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>dsc-carptxt-pgcrw-ltblulrg</t>
+          <t>dsc-calilvcp-nvy/wht</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>California Repeat Text Pigment Dyed Crewneck Light Blue - Large / Pigment Light Blue</t>
+          <t>California Love Flag Flat Bill Snapback Mesh Truckers Cap - Navy/White One Size Fits Most</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -859,27 +859,27 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19896260</v>
+        <v>19896596</v>
       </c>
       <c r="C14" t="n">
         <v>32001378</v>
       </c>
       <c r="D14" t="n">
-        <v>17917476</v>
+        <v>17917773</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>dsc-flgdstrsshdy-med</t>
+          <t>dsc-rchrd-caligldnstate</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>dsc-flgdstrsshdy-med</t>
+          <t>dsc-rchrd-caligldnstate</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>California State Flag Distressed Vintage Asst Colors Hoodie - Medium / Black</t>
+          <t>California Golden State Snapback Trucker Hat - One size fits most / Blue</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -891,27 +891,27 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>19896261</v>
+        <v>19896613</v>
       </c>
       <c r="C15" t="n">
         <v>32001378</v>
       </c>
       <c r="D15" t="n">
-        <v>17917476</v>
+        <v>17917789</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>dsc-carpblkovrsl-rgln-med</t>
+          <t>140524199</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>dsc-carpblkovrsl-rgln-med</t>
+          <t>dsc-DonCRBFlgCRW-red-sm</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>California Republic Black Oversized Silhouette Raglan Hoodie - Medium / Gunmetal Heather/Black</t>
+          <t>California Republic Bear Flag Crewneck Sweatshirt - Red Small</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -923,27 +923,27 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>19896304</v>
+        <v>19896614</v>
       </c>
       <c r="C16" t="n">
         <v>32001378</v>
       </c>
       <c r="D16" t="n">
-        <v>17917518</v>
+        <v>17917790</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>140523888</t>
+          <t>dsc-caliplyngcrd</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>dsc-cr-screenp-trucker-hat-black</t>
+          <t>dsc-caliplyngcrd</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>California Republic Screen Print Trucker Hat - Black</t>
+          <t>California Republic Distressed Design Playing Cards - Default / Cards</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -955,27 +955,27 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>19896305</v>
+        <v>19896621</v>
       </c>
       <c r="C17" t="n">
         <v>32001378</v>
       </c>
       <c r="D17" t="n">
-        <v>17917519</v>
+        <v>17917797</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>dsc-calirpfltcp-blk/wht</t>
+          <t>dsc-rchrd-calisurfco</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>dsc-calirpfltcp-blk/wht</t>
+          <t>dsc-rchrd-calisurfco</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>California Republic Flag Flat Bill Snapback Mesh Truckers Cap - One size fits most / Black/White</t>
+          <t>California Surf Co.Snapback Trucker Hat - One size fits most / Black</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -987,27 +987,27 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>19896306</v>
+        <v>19896622</v>
       </c>
       <c r="C18" t="n">
         <v>32001378</v>
       </c>
       <c r="D18" t="n">
-        <v>17917519</v>
+        <v>17917798</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>dsc-caliorg-fb-blk</t>
+          <t>140524210</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>dsc-caliorg-fb-blk</t>
+          <t>dsc-DonCRBFlgTNK-sprtgryxxl</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>California Republic Original State Flag Snapback Hat On Black - Flat Bill - One size fits most / Black/White</t>
+          <t>California Republic Bear Flag Tank Top - Sport Grey XX-Large</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1019,27 +1019,27 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>19896319</v>
+        <v>19896627</v>
       </c>
       <c r="C19" t="n">
         <v>32001378</v>
       </c>
       <c r="D19" t="n">
-        <v>17917531</v>
+        <v>17917802</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>dsc-trkrcp-blk/wht</t>
+          <t>140524215</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>dsc-trkrcp-blk/wht</t>
+          <t>dsc-athstht-drkblu-smmd</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>California State Flag Snapback Mesh Truckers Cap - One size fits most / Black/White</t>
+          <t>Atheist Offset Symbol Curved Bill Baseball Hat Flexfit-Dark Grey SM/MD</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1051,27 +1051,27 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>19896428</v>
+        <v>19896629</v>
       </c>
       <c r="C20" t="n">
         <v>32001378</v>
       </c>
       <c r="D20" t="n">
-        <v>17917627</v>
+        <v>17917804</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>dsc-casnglepoppy-kychn</t>
+          <t>140524217</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>dsc-casnglepoppy-kychn</t>
+          <t>dsc-CRVntgStrpPRMYTHHDY-gryhthrlrg</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>California Single Poppy Keychain - One Size / One Color</t>
+          <t>California Republic Vintage Stripe Premium Youth Sweatshirt Hoodie - Grey Heather Large</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1083,27 +1083,27 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>19896429</v>
+        <v>19896636</v>
       </c>
       <c r="C21" t="n">
         <v>32001378</v>
       </c>
       <c r="D21" t="n">
-        <v>17917627</v>
+        <v>17917811</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>ClGldnSttHbscsPRM2500-DstyRslrg</t>
+          <t>DnPmntlCalRpBlkTxt-SDTEE-HthrOlvxlg</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>ClGldnSttHbscsPRM2500-DstyRslrg</t>
+          <t>DnPmntlCalRpBlkTxt-SDTEE-HthrOlvxlg</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Cali Golden State Hibiscus Women's Soft Hooded Pullover - Large / Dusty Rose</t>
+          <t>Don Pimentel California Republic Bear Flag Black Text Asst Colors Sueded Tee - X-Large / Heather Olive</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1115,27 +1115,27 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>19896430</v>
+        <v>19896656</v>
       </c>
       <c r="C22" t="n">
         <v>32001378</v>
       </c>
       <c r="D22" t="n">
-        <v>17917627</v>
+        <v>17917829</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Rube3PRM2500-MstyBlulrg</t>
+          <t>sf-calihugcrds</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Rube3PRM2500-MstyBlulrg</t>
+          <t>sf-calihugcrds</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>California Poppies Green Text Women's Soft Hooded Pullover - Large / Misty Blue</t>
+          <t>California Bear Hug Playing Cards - Default / Cards</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1147,27 +1147,27 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>19896431</v>
+        <v>19896662</v>
       </c>
       <c r="C23" t="n">
         <v>32001378</v>
       </c>
       <c r="D23" t="n">
-        <v>17917627</v>
+        <v>17917834</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>ClGldnStHbscsWmRlxJrsTee-hthrsnst-lrg</t>
+          <t>dsc-whang-teal-purple-white</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>ClGldnStHbscsWmRlxJrsTee-hthrsnst-lrg</t>
+          <t>dsc-whang-teal-purple-white</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Cali Golden State Hibiscus Women's Relaxed Jersey Tee - Large / Heather Sunset</t>
+          <t>California Republic Cali State Bear Flag Snapback Hat Teal Purple White by Whang - One size fits most / White</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1179,27 +1179,27 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>19896432</v>
+        <v>19896661</v>
       </c>
       <c r="C24" t="n">
         <v>32001378</v>
       </c>
       <c r="D24" t="n">
-        <v>17917627</v>
+        <v>17917835</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>CalRpcPlmTrs-SDTEE-BlkHthrlrg</t>
+          <t>dsc-ClfrnVntgStrpZU-chhthxxl</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>CalRpcPlmTrs-SDTEE-BlkHthrlrg</t>
+          <t>dsc-ClfrnVntgStrpZU-chhthxxl</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>California Republic Palm Trees Asst Colors Sueded Tee - Large / Black Heather</t>
+          <t>California Vintage Stripe Zip-Up Hoodie - XX-Large / Charcoal Heather</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1211,27 +1211,27 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>19896433</v>
+        <v>19896681</v>
       </c>
       <c r="C25" t="n">
         <v>32001378</v>
       </c>
       <c r="D25" t="n">
-        <v>17917627</v>
+        <v>17917852</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>CalRpcPlmTrs-SDTEE-HthrPchlrg</t>
+          <t>140524270</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>CalRpcPlmTrs-SDTEE-HthrPchlrg</t>
+          <t>dsc-casnglepoppy-kychn</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>California Republic Palm Trees Asst Colors Sueded Tee - Large / Heather Peach</t>
+          <t>California Single Poppy Keychain</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1243,27 +1243,27 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>19896477</v>
+        <v>19896723</v>
       </c>
       <c r="C26" t="n">
         <v>32001378</v>
       </c>
       <c r="D26" t="n">
-        <v>17917666</v>
+        <v>17917885</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>dsc-rtrobldtee-mrnxlg</t>
+          <t>dsc-calihat-blk-lrgxlg</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>dsc-rtrobldtee-mrnxlg</t>
+          <t>dsc-calihat-blk-lrgxlg</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>California Republic Vintage Retro Asst Colors T-shirt/tee - X-Large / Maroon</t>
+          <t>California Flag Flexfit Baseball Hat - Large/X-Large / Black</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1275,27 +1275,27 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>19896479</v>
+        <v>19896740</v>
       </c>
       <c r="C27" t="n">
         <v>32001378</v>
       </c>
       <c r="D27" t="n">
-        <v>17917668</v>
+        <v>17917902</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>140524065</t>
+          <t>dsc-calamrflg-TrnsfMNSTEE-whtlrg</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>dsc-CalNo1DmndHDY-rshgrnxxl</t>
+          <t>dsc-calamrflg-TrnsfMNSTEE-whtlrg</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>California Republic No. 1 Diamond Hustle Sweatshirt Hoodie - Irish Green XX-Large</t>
+          <t>American Bear Flag Asst Colors Mens Lightweight Fitted T-Shirt/tee - Large / White</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1307,27 +1307,27 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>19896528</v>
+        <v>19896741</v>
       </c>
       <c r="C28" t="n">
         <v>32001378</v>
       </c>
       <c r="D28" t="n">
-        <v>17917713</v>
+        <v>17917903</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>CaRpBrdrlssBrFlgSPRSFTCRW-mstblu-xl</t>
+          <t>dsc-libertyogretro</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>CaRpBrdrlssBrFlgSPRSFTCRW-mstblu-xl</t>
+          <t>dsc-libertyogretro</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>California Republic Borderless Bear Flag Super Soft Crewneck Sweater - X-Large / Misty Blue</t>
+          <t>California Republic Original Retro Cotton Canvas Drawstring Backpack - One-Size / Black</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1339,27 +1339,27 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>19896578</v>
+        <v>19896743</v>
       </c>
       <c r="C29" t="n">
         <v>32001378</v>
       </c>
       <c r="D29" t="n">
-        <v>17917757</v>
+        <v>17917905</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>140524164</t>
+          <t>dsc-whang-Cord-Blk</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>dsc-capoppystckr</t>
+          <t>dsc-whang-Cord-Blk</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Life at Sea Sticker (CA Poppy)</t>
+          <t>New CALIFORNIA REPUBLIC CORDUROY SNAPBACK HAT - Black - One size fits most / Black</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1371,31 +1371,31 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>19896579</v>
+        <v>19896777</v>
       </c>
       <c r="C30" t="n">
         <v>32001378</v>
       </c>
       <c r="D30" t="n">
-        <v>17917758</v>
+        <v>17917938</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>140524165</t>
+          <t>sf-poppyorn</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>dsc-calilvcp-nvy/wht</t>
+          <t>sf-poppyorn</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>California Love Flag Flat Bill Snapback Mesh Truckers Cap - Navy/White One Size Fits Most</t>
+          <t>California Golden Poppy Glass Ornament - Standard / Yellow</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -1403,27 +1403,27 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>19896596</v>
+        <v>19896779</v>
       </c>
       <c r="C31" t="n">
         <v>32001378</v>
       </c>
       <c r="D31" t="n">
-        <v>17917773</v>
+        <v>17917940</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>dsc-rchrd-caligldnstate</t>
+          <t>dsc-flgdstrsshdy-sml</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>dsc-rchrd-caligldnstate</t>
+          <t>dsc-flgdstrsshdy-sml</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>California Golden State Snapback Trucker Hat - One size fits most / Blue</t>
+          <t>California State Flag Distressed Vintage Asst Colors Hoodie - Small / Black</t>
         </is>
       </c>
       <c r="H31" t="n">
@@ -1435,27 +1435,27 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>19896613</v>
+        <v>19896784</v>
       </c>
       <c r="C32" t="n">
         <v>32001378</v>
       </c>
       <c r="D32" t="n">
-        <v>17917789</v>
+        <v>17917945</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>140524199</t>
+          <t>dsc-dsc-mmsig-redlrg</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>dsc-DonCRBFlgCRW-red-sm</t>
+          <t>dsc-dsc-mmsig-redlrg</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>California Republic Bear Flag Crewneck Sweatshirt - Red Small</t>
+          <t>Marilyn Monroe Portrait Signature Asst Colors T-shirt/tee - Large / Red</t>
         </is>
       </c>
       <c r="H32" t="n">
@@ -1467,27 +1467,27 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>19896614</v>
+        <v>19896787</v>
       </c>
       <c r="C33" t="n">
         <v>32001378</v>
       </c>
       <c r="D33" t="n">
-        <v>17917790</v>
+        <v>17917948</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>dsc-caliplyngcrd</t>
+          <t>140524376</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>dsc-caliplyngcrd</t>
+          <t>dsc-cgirl-trucker-blackbluestitch</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>California Republic Distressed Design Playing Cards - Default / Cards</t>
+          <t>California Girl Trucker Snapback Hat - Black/White</t>
         </is>
       </c>
       <c r="H33" t="n">
@@ -1499,27 +1499,27 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>19896621</v>
+        <v>19896806</v>
       </c>
       <c r="C34" t="n">
         <v>32001378</v>
       </c>
       <c r="D34" t="n">
-        <v>17917797</v>
+        <v>17917967</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>dsc-rchrd-calisurfco</t>
+          <t>dsc-OctheattrnsfrLS-ryllrg</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>dsc-rchrd-calisurfco</t>
+          <t>dsc-OctheattrnsfrLS-ryllrg</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>California Surf Co.Snapback Trucker Hat - One size fits most / Black</t>
+          <t>Octopus Long Sleeve Shirt - Large / Royal</t>
         </is>
       </c>
       <c r="H34" t="n">
@@ -1531,27 +1531,27 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>19896622</v>
+        <v>19896812</v>
       </c>
       <c r="C35" t="n">
         <v>32001378</v>
       </c>
       <c r="D35" t="n">
-        <v>17917798</v>
+        <v>17917973</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>140524210</t>
+          <t>dsc-calvancp-blk</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>dsc-DonCRBFlgTNK-sprtgryxxl</t>
+          <t>dsc-calvancp-blk</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>California Republic Bear Flag Tank Top - Sport Grey XX-Large</t>
+          <t>California Republic Vintage Van Snapback Mesh Truckers Cap - Black One Size Fits Most - One size fits most / Black</t>
         </is>
       </c>
       <c r="H35" t="n">
@@ -1563,27 +1563,27 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>19896627</v>
+        <v>19896823</v>
       </c>
       <c r="C36" t="n">
         <v>32001378</v>
       </c>
       <c r="D36" t="n">
-        <v>17917802</v>
+        <v>17917981</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>140524215</t>
+          <t>dsc-ClfrnVntgStrpZU-blksml</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>dsc-athstht-drkblu-smmd</t>
+          <t>dsc-ClfrnVntgStrpZU-blksml</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Atheist Offset Symbol Curved Bill Baseball Hat Flexfit-Dark Grey SM/MD</t>
+          <t>California Vintage Stripe Zip-Up Hoodie - Small / Black</t>
         </is>
       </c>
       <c r="H36" t="n">
@@ -1595,27 +1595,27 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>19896629</v>
+        <v>19896824</v>
       </c>
       <c r="C37" t="n">
         <v>32001378</v>
       </c>
       <c r="D37" t="n">
-        <v>17917804</v>
+        <v>17917982</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>140524217</t>
+          <t>140524414</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>dsc-CRVntgStrpPRMYTHHDY-gryhthrlrg</t>
+          <t>dsc-CalNo1Dmnd-hthrspphxlg</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>California Republic Vintage Stripe Premium Youth Sweatshirt Hoodie - Grey Heather Large</t>
+          <t>California Republic No. 1 Diamond Hustle T-shirt/tee - Heather Sapphire X-Large</t>
         </is>
       </c>
       <c r="H37" t="n">
@@ -1627,27 +1627,27 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>19896636</v>
+        <v>19896825</v>
       </c>
       <c r="C38" t="n">
         <v>32001378</v>
       </c>
       <c r="D38" t="n">
-        <v>17917811</v>
+        <v>17917982</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>DnPmntlCalRpBlkTxt-SDTEE-HthrOlvxlg</t>
+          <t>140524415</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>DnPmntlCalRpBlkTxt-SDTEE-HthrOlvxlg</t>
+          <t>dsc-CalNo1Dmnd-crdrdxlg</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Don Pimentel California Republic Bear Flag Black Text Asst Colors Sueded Tee - X-Large / Heather Olive</t>
+          <t>California Republic No. 1 Diamond Hustle T-shirt/tee - Cardinal Red X-Large</t>
         </is>
       </c>
       <c r="H38" t="n">
@@ -1659,27 +1659,27 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>19896656</v>
+        <v>19896826</v>
       </c>
       <c r="C39" t="n">
         <v>32001378</v>
       </c>
       <c r="D39" t="n">
-        <v>17917829</v>
+        <v>17917983</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>sf-calihugcrds</t>
+          <t>dsc-CrsMnDrmctrWht-blkxlg</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>sf-calihugcrds</t>
+          <t>dsc-CrsMnDrmctrWht-blkxlg</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>California Bear Hug Playing Cards - Default / Cards</t>
+          <t>Crescent Moon Dreamcatcher White Asst Colors T-shirt/tee - X-Large / Black</t>
         </is>
       </c>
       <c r="H39" t="n">
@@ -1691,27 +1691,27 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>19896662</v>
+        <v>19896830</v>
       </c>
       <c r="C40" t="n">
         <v>32001378</v>
       </c>
       <c r="D40" t="n">
-        <v>17917834</v>
+        <v>17917987</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>dsc-whang-teal-purple-white</t>
+          <t>sf-cabearhugcstrs</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>dsc-whang-teal-purple-white</t>
+          <t>sf-cabearhugcstrs</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>California Republic Cali State Bear Flag Snapback Hat Teal Purple White by Whang - One size fits most / White</t>
+          <t>California Bear Hug Coasters set of 4 - Standard / brown</t>
         </is>
       </c>
       <c r="H40" t="n">
@@ -1723,27 +1723,27 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>19896661</v>
+        <v>19896839</v>
       </c>
       <c r="C41" t="n">
         <v>32001378</v>
       </c>
       <c r="D41" t="n">
-        <v>17917835</v>
+        <v>17917996</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>dsc-ClfrnVntgStrpZU-chhthxxl</t>
+          <t>dsc-ClfrnVntgStrpZU-blksml</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>dsc-ClfrnVntgStrpZU-chhthxxl</t>
+          <t>dsc-ClfrnVntgStrpZU-blksml</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>California Vintage Stripe Zip-Up Hoodie - XX-Large / Charcoal Heather</t>
+          <t>California Vintage Stripe Zip-Up Hoodie - Small / Black</t>
         </is>
       </c>
       <c r="H41" t="n">
@@ -1755,30 +1755,158 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>19896681</v>
+        <v>19896844</v>
       </c>
       <c r="C42" t="n">
         <v>32001378</v>
       </c>
       <c r="D42" t="n">
-        <v>17917852</v>
+        <v>17918000</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>140524270</t>
+          <t>140524434</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>dsc-casnglepoppy-kychn</t>
+          <t>dsc-lrgtote</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>California Single Poppy Keychain</t>
+          <t>California Republic Recycled Shopping Tote Bag - Large Size</t>
         </is>
       </c>
       <c r="H42" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>19896851</v>
+      </c>
+      <c r="C43" t="n">
+        <v>32001378</v>
+      </c>
+      <c r="D43" t="n">
+        <v>17918007</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>140524441</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>sf-TeaTwl</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>I Love You California Tea Towel</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>19896852</v>
+      </c>
+      <c r="C44" t="n">
+        <v>32001378</v>
+      </c>
+      <c r="D44" t="n">
+        <v>17918008</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>dsc-brdlss-blklrg</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>dsc-brdlss-blklrg</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>California State Flag Borderless Asst Colors T-shirt/tee - Large / Black</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>19896853</v>
+      </c>
+      <c r="C45" t="n">
+        <v>32001378</v>
+      </c>
+      <c r="D45" t="n">
+        <v>17918009</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>140524443</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>ClfrnClsscSnrsSrfngPRM2500-Blshxxl</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>California Classic Sunrise Surfing Women's Soft Hooded Pullover - Blush XX-Large</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>19896858</v>
+      </c>
+      <c r="C46" t="n">
+        <v>32001378</v>
+      </c>
+      <c r="D46" t="n">
+        <v>17918014</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>dsc-ClfrnVntgStrpZU-blkmed</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>dsc-ClfrnVntgStrpZU-blkmed</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>California Vintage Stripe Zip-Up Hoodie - Medium / Black</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>